<commit_message>
removed embedded resource from cs file project
also added the datacenter xls template file to the git ignore
</commit_message>
<xml_diff>
--- a/dataCenter.xlsx
+++ b/dataCenter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filipe.cacho\Documents\MY  CODE\RitmsHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E12CFD-5258-40D2-BBC2-767BC3A77C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04BD136-FA97-43C8-9D49-20F3660224DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DF524610-1964-40D8-A05C-F2A29F859B9B}"/>
+    <workbookView xWindow="4110" yWindow="3525" windowWidth="21600" windowHeight="11295" xr2:uid="{DF524610-1964-40D8-A05C-F2A29F859B9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>https://edprdesarrollo1.crm4.dynamics.com/</t>
   </si>
@@ -149,13 +149,19 @@
   </si>
   <si>
     <t>yourpass</t>
+  </si>
+  <si>
+    <t>ex121935@edpr.com</t>
+  </si>
+  <si>
+    <t>EDPAuth201..18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +194,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,9 +220,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -227,17 +242,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{DA41252F-8B8F-4D2D-8A79-C889F3F50354}"/>
   </cellStyles>
@@ -573,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762D61FB-AE8E-4157-B830-B7F5ECF54A7B}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +636,7 @@
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -646,7 +662,7 @@
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -672,11 +688,11 @@
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>35</v>
+      <c r="B4" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>17</v>
@@ -696,8 +712,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{FBD9B027-8C50-4CB0-B260-0C48397F8924}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -705,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587A5E4A-68E0-4D45-BDD1-D8521CA067EB}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -801,26 +820,26 @@
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>